<commit_message>
aggiunta regressione lineare e multipla
</commit_message>
<xml_diff>
--- a/Progetto_SAD/utenti_per_regione_e_anno.xlsx
+++ b/Progetto_SAD/utenti_per_regione_e_anno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\git\Progetto_SAD\Progetto_SAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B0BBBE-4B19-4E80-A29C-24DF8B440214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E3D9D4-6995-407D-B700-2671D5E69232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -209,6 +209,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -525,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,35 +1206,35 @@
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <f>SUM(B2:B23)/COUNT(B2:B23)</f>
         <v>473.59090909090907</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <f t="shared" ref="C24:I24" si="0">SUM(C2:C23)/COUNT(C2:C23)</f>
         <v>395.77272727272725</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <f t="shared" si="0"/>
         <v>282.04545454545456</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="7">
         <f t="shared" si="0"/>
         <v>253.27272727272728</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="7">
         <f t="shared" si="0"/>
         <v>207.81818181818181</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="7">
         <f t="shared" si="0"/>
         <v>298.59090909090907</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="7">
         <f t="shared" si="0"/>
         <v>291.09090909090907</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="7">
         <f t="shared" si="0"/>
         <v>569.77272727272725</v>
       </c>
@@ -1251,6 +1252,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EF10C102774CC343B14B44E209154F29" ma:contentTypeVersion="2" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="bc2ec9980fa900ddddaa9f057be1b905">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e86a63c2-7291-4cd2-9ba5-95d203bf00ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c4c5a164cc73ae35ac9b7fd0b262a4c" ns2:_="">
     <xsd:import namespace="e86a63c2-7291-4cd2-9ba5-95d203bf00ef"/>
@@ -1382,15 +1392,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F9E433-AE66-48A8-A4C7-CE845E54A75C}">
   <ds:schemaRefs>
@@ -1408,6 +1409,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DCFCD5-E974-4F89-A09E-AB92BF13F64D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C3148-61F8-42CE-8EEC-9B882D8A0DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1423,12 +1432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DCFCD5-E974-4F89-A09E-AB92BF13F64D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
devo fare i cluster
</commit_message>
<xml_diff>
--- a/Progetto_SAD/utenti_per_regione_e_anno.xlsx
+++ b/Progetto_SAD/utenti_per_regione_e_anno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\git\Progetto_SAD\Progetto_SAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E3D9D4-6995-407D-B700-2671D5E69232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8FFD68-B5FB-4457-B9BA-090CA3F3BDD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +128,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -210,6 +218,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -524,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +544,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -564,7 +573,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,7 +602,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -622,7 +631,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -651,7 +660,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -680,7 +689,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -709,7 +718,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -738,7 +747,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -767,7 +776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -796,7 +805,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -824,8 +833,9 @@
       <c r="I10" s="4">
         <v>163</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -854,7 +864,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -883,7 +893,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -912,7 +922,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -941,7 +951,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -970,7 +980,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>473.59090909090907</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" ref="C24:I24" si="0">SUM(C2:C23)/COUNT(C2:C23)</f>
+        <f t="shared" ref="C24:G24" si="0">SUM(C2:C23)/COUNT(C2:C23)</f>
         <v>395.77272727272725</v>
       </c>
       <c r="D24" s="7">
@@ -1231,11 +1241,11 @@
         <v>298.59090909090907</v>
       </c>
       <c r="H24" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(H2:H23)/COUNT(H2:H23)</f>
         <v>291.09090909090907</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(I2:I23)/COUNT(I2:I23)</f>
         <v>569.77272727272725</v>
       </c>
     </row>
@@ -1246,21 +1256,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EF10C102774CC343B14B44E209154F29" ma:contentTypeVersion="2" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="bc2ec9980fa900ddddaa9f057be1b905">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e86a63c2-7291-4cd2-9ba5-95d203bf00ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c4c5a164cc73ae35ac9b7fd0b262a4c" ns2:_="">
     <xsd:import namespace="e86a63c2-7291-4cd2-9ba5-95d203bf00ef"/>
@@ -1392,31 +1387,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F9E433-AE66-48A8-A4C7-CE845E54A75C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e86a63c2-7291-4cd2-9ba5-95d203bf00ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DCFCD5-E974-4F89-A09E-AB92BF13F64D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C3148-61F8-42CE-8EEC-9B882D8A0DA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1432,4 +1418,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DCFCD5-E974-4F89-A09E-AB92BF13F64D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F9E433-AE66-48A8-A4C7-CE845E54A75C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e86a63c2-7291-4cd2-9ba5-95d203bf00ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>